<commit_message>
Simplified data processing and added YPD data
</commit_message>
<xml_diff>
--- a/Datasets/12140549/raw_data/phenotype_mapping.xlsx
+++ b/Datasets/12140549/raw_data/phenotype_mapping.xlsx
@@ -1,16 +1,24 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="22810"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="5" rupBuild="27809"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/abaryshnikova/Lab/Projects/Phenotypes/Yeastphenome.org-Loading-data/Datasets/12140549/raw_data/"/>
+    </mc:Choice>
+  </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="56420" yWindow="5280" windowWidth="25600" windowHeight="18380" tabRatio="500"/>
+    <workbookView xWindow="-33940" yWindow="4000" windowWidth="25600" windowHeight="18380" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
   <calcPr calcId="140000" concurrentCalc="0"/>
   <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{79F54976-1DA5-4618-B147-4CDE4B953A38}">
+      <x14:workbookPr defaultImageDpi="32767"/>
+    </ext>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{7523E5D3-25F3-A5E0-1632-64F254C22452}">
       <mx:ArchID Flags="2"/>
     </ext>
@@ -19,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="226" uniqueCount="52">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="227" uniqueCount="53">
   <si>
     <t>barcode microarray hydridization</t>
   </si>
@@ -175,6 +183,9 @@
   </si>
   <si>
     <t>Experiment</t>
+  </si>
+  <si>
+    <t>Dataset id</t>
   </si>
 </sst>
 </file>
@@ -235,6 +246,11 @@
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleMedium4"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
+      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+  </extLst>
 </styleSheet>
 </file>
 
@@ -560,952 +576,1043 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:I32"/>
+  <dimension ref="A1:J32"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C15" sqref="C15"/>
+      <selection activeCell="B2" sqref="B2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="2" max="2" width="28" customWidth="1"/>
-    <col min="3" max="3" width="29.1640625" customWidth="1"/>
+    <col min="3" max="3" width="28" customWidth="1"/>
+    <col min="4" max="4" width="29.1640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9">
+    <row r="1" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A1" s="2" t="s">
         <v>51</v>
       </c>
       <c r="B1" s="2" t="s">
+        <v>52</v>
+      </c>
+      <c r="C1" s="2" t="s">
         <v>50</v>
       </c>
-      <c r="C1" s="2" t="s">
+      <c r="D1" s="2" t="s">
         <v>49</v>
       </c>
-      <c r="D1" s="2" t="s">
+      <c r="E1" s="2" t="s">
         <v>48</v>
       </c>
-      <c r="E1" s="2" t="s">
+      <c r="F1" s="2" t="s">
         <v>47</v>
       </c>
-      <c r="F1" s="2" t="s">
+      <c r="G1" s="2" t="s">
         <v>46</v>
       </c>
-      <c r="G1" s="2" t="s">
+      <c r="H1" s="2" t="s">
         <v>45</v>
       </c>
-      <c r="H1" s="2" t="s">
+      <c r="I1" s="2" t="s">
         <v>44</v>
       </c>
-      <c r="I1" s="2" t="s">
+      <c r="J1" s="2" t="s">
         <v>43</v>
       </c>
     </row>
-    <row r="2" spans="1:9">
+    <row r="2" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A2">
         <v>48</v>
       </c>
-      <c r="B2" t="s">
+      <c r="B2">
+        <v>712</v>
+      </c>
+      <c r="C2" t="s">
         <v>15</v>
       </c>
-      <c r="C2" t="s">
+      <c r="D2" t="s">
         <v>42</v>
       </c>
-      <c r="D2" t="s">
+      <c r="E2" t="s">
         <v>38</v>
       </c>
-      <c r="E2">
+      <c r="F2">
         <v>13</v>
       </c>
-      <c r="F2" t="s">
+      <c r="G2" t="s">
         <v>13</v>
       </c>
-      <c r="G2" t="s">
-        <v>2</v>
-      </c>
       <c r="H2" t="s">
-        <v>1</v>
-      </c>
-      <c r="I2" s="1" t="s">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="3" spans="1:9">
+        <v>2</v>
+      </c>
+      <c r="I2" t="s">
+        <v>1</v>
+      </c>
+      <c r="J2" s="1" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="3" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A3">
         <v>45</v>
       </c>
-      <c r="B3" t="s">
+      <c r="B3">
+        <v>712</v>
+      </c>
+      <c r="C3" t="s">
         <v>15</v>
       </c>
-      <c r="C3" t="s">
+      <c r="D3" t="s">
         <v>41</v>
       </c>
-      <c r="D3" t="s">
+      <c r="E3" t="s">
         <v>38</v>
       </c>
-      <c r="E3">
+      <c r="F3">
         <v>13</v>
       </c>
-      <c r="F3" t="s">
+      <c r="G3" t="s">
         <v>13</v>
       </c>
-      <c r="G3" t="s">
-        <v>2</v>
-      </c>
       <c r="H3" t="s">
-        <v>1</v>
-      </c>
-      <c r="I3" s="1" t="s">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="4" spans="1:9">
+        <v>2</v>
+      </c>
+      <c r="I3" t="s">
+        <v>1</v>
+      </c>
+      <c r="J3" s="1" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="4" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A4">
         <v>14</v>
       </c>
-      <c r="B4" t="s">
-        <v>6</v>
+      <c r="B4">
+        <v>717</v>
       </c>
       <c r="C4" t="s">
+        <v>6</v>
+      </c>
+      <c r="D4" t="s">
         <v>40</v>
       </c>
-      <c r="D4" t="s">
+      <c r="E4" t="s">
         <v>38</v>
       </c>
-      <c r="E4">
+      <c r="F4">
         <v>13</v>
       </c>
-      <c r="F4" t="s">
-        <v>3</v>
-      </c>
       <c r="G4" t="s">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="H4" t="s">
-        <v>1</v>
-      </c>
-      <c r="I4" s="1" t="s">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="5" spans="1:9">
+        <v>2</v>
+      </c>
+      <c r="I4" t="s">
+        <v>1</v>
+      </c>
+      <c r="J4" s="1" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="5" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A5">
         <v>10</v>
       </c>
-      <c r="B5" t="s">
-        <v>6</v>
+      <c r="B5">
+        <v>717</v>
       </c>
       <c r="C5" t="s">
+        <v>6</v>
+      </c>
+      <c r="D5" t="s">
         <v>39</v>
       </c>
-      <c r="D5" t="s">
+      <c r="E5" t="s">
         <v>38</v>
       </c>
-      <c r="E5">
+      <c r="F5">
         <v>13</v>
       </c>
-      <c r="F5" t="s">
-        <v>3</v>
-      </c>
       <c r="G5" t="s">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="H5" t="s">
-        <v>1</v>
-      </c>
-      <c r="I5" s="1" t="s">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="6" spans="1:9">
+        <v>2</v>
+      </c>
+      <c r="I5" t="s">
+        <v>1</v>
+      </c>
+      <c r="J5" s="1" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="6" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A6">
         <v>46</v>
       </c>
-      <c r="B6" t="s">
+      <c r="B6">
+        <v>713</v>
+      </c>
+      <c r="C6" t="s">
         <v>15</v>
       </c>
-      <c r="C6" t="s">
+      <c r="D6" t="s">
         <v>37</v>
       </c>
-      <c r="D6" t="s">
-        <v>4</v>
-      </c>
-      <c r="E6">
+      <c r="E6" t="s">
+        <v>4</v>
+      </c>
+      <c r="F6">
         <v>185</v>
       </c>
-      <c r="F6" t="s">
+      <c r="G6" t="s">
         <v>13</v>
       </c>
-      <c r="G6" t="s">
-        <v>2</v>
-      </c>
       <c r="H6" t="s">
-        <v>1</v>
-      </c>
-      <c r="I6" s="1" t="s">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="7" spans="1:9">
+        <v>2</v>
+      </c>
+      <c r="I6" t="s">
+        <v>1</v>
+      </c>
+      <c r="J6" s="1" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="7" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A7">
         <v>31</v>
       </c>
-      <c r="B7" t="s">
+      <c r="B7">
+        <v>713</v>
+      </c>
+      <c r="C7" t="s">
         <v>29</v>
       </c>
-      <c r="C7" t="s">
+      <c r="D7" t="s">
         <v>36</v>
       </c>
-      <c r="D7" t="s">
-        <v>4</v>
-      </c>
-      <c r="E7">
+      <c r="E7" t="s">
+        <v>4</v>
+      </c>
+      <c r="F7">
         <v>185</v>
       </c>
-      <c r="F7" t="s">
+      <c r="G7" t="s">
         <v>13</v>
       </c>
-      <c r="G7" t="s">
-        <v>2</v>
-      </c>
       <c r="H7" t="s">
-        <v>1</v>
-      </c>
-      <c r="I7" s="1" t="s">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="8" spans="1:9">
+        <v>2</v>
+      </c>
+      <c r="I7" t="s">
+        <v>1</v>
+      </c>
+      <c r="J7" s="1" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="8" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A8">
         <v>11</v>
       </c>
-      <c r="B8" t="s">
-        <v>6</v>
+      <c r="B8">
+        <v>716</v>
       </c>
       <c r="C8" t="s">
+        <v>6</v>
+      </c>
+      <c r="D8" t="s">
         <v>35</v>
       </c>
-      <c r="D8" t="s">
-        <v>4</v>
-      </c>
-      <c r="E8">
+      <c r="E8" t="s">
+        <v>4</v>
+      </c>
+      <c r="F8">
         <v>185</v>
       </c>
-      <c r="F8" t="s">
-        <v>3</v>
-      </c>
       <c r="G8" t="s">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="H8" t="s">
-        <v>1</v>
-      </c>
-      <c r="I8" s="1" t="s">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="9" spans="1:9">
+        <v>2</v>
+      </c>
+      <c r="I8" t="s">
+        <v>1</v>
+      </c>
+      <c r="J8" s="1" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="9" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A9">
         <v>13</v>
       </c>
-      <c r="B9" t="s">
-        <v>6</v>
+      <c r="B9">
+        <v>716</v>
       </c>
       <c r="C9" t="s">
+        <v>6</v>
+      </c>
+      <c r="D9" t="s">
         <v>34</v>
       </c>
-      <c r="D9" t="s">
-        <v>4</v>
-      </c>
-      <c r="E9">
+      <c r="E9" t="s">
+        <v>4</v>
+      </c>
+      <c r="F9">
         <v>185</v>
       </c>
-      <c r="F9" t="s">
-        <v>3</v>
-      </c>
       <c r="G9" t="s">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="H9" t="s">
-        <v>1</v>
-      </c>
-      <c r="I9" s="1" t="s">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="10" spans="1:9">
+        <v>2</v>
+      </c>
+      <c r="I9" t="s">
+        <v>1</v>
+      </c>
+      <c r="J9" s="1" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="10" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A10">
         <v>19</v>
       </c>
-      <c r="B10" t="s">
+      <c r="B10">
+        <v>472</v>
+      </c>
+      <c r="C10" t="s">
         <v>15</v>
       </c>
-      <c r="C10" t="s">
+      <c r="D10" t="s">
         <v>33</v>
       </c>
-      <c r="D10" t="s">
-        <v>4</v>
-      </c>
-      <c r="E10">
+      <c r="E10" t="s">
+        <v>4</v>
+      </c>
+      <c r="F10">
         <v>517</v>
       </c>
-      <c r="F10" t="s">
+      <c r="G10" t="s">
         <v>13</v>
       </c>
-      <c r="G10" t="s">
-        <v>2</v>
-      </c>
       <c r="H10" t="s">
-        <v>1</v>
-      </c>
-      <c r="I10" s="1" t="s">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="11" spans="1:9">
+        <v>2</v>
+      </c>
+      <c r="I10" t="s">
+        <v>1</v>
+      </c>
+      <c r="J10" s="1" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="11" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A11">
         <v>18</v>
       </c>
-      <c r="B11" t="s">
+      <c r="B11">
+        <v>472</v>
+      </c>
+      <c r="C11" t="s">
         <v>15</v>
       </c>
-      <c r="C11" t="s">
+      <c r="D11" t="s">
         <v>32</v>
       </c>
-      <c r="D11" t="s">
-        <v>4</v>
-      </c>
-      <c r="E11">
+      <c r="E11" t="s">
+        <v>4</v>
+      </c>
+      <c r="F11">
         <v>517</v>
       </c>
-      <c r="F11" t="s">
+      <c r="G11" t="s">
         <v>13</v>
       </c>
-      <c r="G11" t="s">
-        <v>2</v>
-      </c>
       <c r="H11" t="s">
-        <v>1</v>
-      </c>
-      <c r="I11" s="1" t="s">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="12" spans="1:9">
+        <v>2</v>
+      </c>
+      <c r="I11" t="s">
+        <v>1</v>
+      </c>
+      <c r="J11" s="1" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="12" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A12">
         <v>5</v>
       </c>
-      <c r="B12" t="s">
-        <v>6</v>
+      <c r="B12">
+        <v>714</v>
       </c>
       <c r="C12" t="s">
+        <v>6</v>
+      </c>
+      <c r="D12" t="s">
         <v>31</v>
       </c>
-      <c r="D12" t="s">
-        <v>4</v>
-      </c>
-      <c r="E12">
+      <c r="E12" t="s">
+        <v>4</v>
+      </c>
+      <c r="F12">
         <v>517</v>
       </c>
-      <c r="F12" t="s">
-        <v>3</v>
-      </c>
       <c r="G12" t="s">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="H12" t="s">
-        <v>1</v>
-      </c>
-      <c r="I12" s="1" t="s">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="13" spans="1:9">
+        <v>2</v>
+      </c>
+      <c r="I12" t="s">
+        <v>1</v>
+      </c>
+      <c r="J12" s="1" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="13" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A13">
         <v>3</v>
       </c>
-      <c r="B13" t="s">
-        <v>6</v>
+      <c r="B13">
+        <v>714</v>
       </c>
       <c r="C13" t="s">
+        <v>6</v>
+      </c>
+      <c r="D13" t="s">
         <v>30</v>
       </c>
-      <c r="D13" t="s">
-        <v>4</v>
-      </c>
-      <c r="E13">
+      <c r="E13" t="s">
+        <v>4</v>
+      </c>
+      <c r="F13">
         <v>517</v>
       </c>
-      <c r="F13" t="s">
-        <v>3</v>
-      </c>
       <c r="G13" t="s">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="H13" t="s">
-        <v>1</v>
-      </c>
-      <c r="I13" s="1" t="s">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="14" spans="1:9">
+        <v>2</v>
+      </c>
+      <c r="I13" t="s">
+        <v>1</v>
+      </c>
+      <c r="J13" s="1" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="14" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A14">
         <v>29</v>
       </c>
-      <c r="B14" t="s">
+      <c r="B14">
+        <v>710</v>
+      </c>
+      <c r="C14" t="s">
         <v>29</v>
       </c>
-      <c r="C14" t="s">
+      <c r="D14" t="s">
         <v>28</v>
       </c>
-      <c r="D14" t="s">
+      <c r="E14" t="s">
         <v>24</v>
       </c>
-      <c r="E14">
+      <c r="F14">
         <v>518</v>
       </c>
-      <c r="F14" t="s">
+      <c r="G14" t="s">
         <v>13</v>
       </c>
-      <c r="G14" t="s">
-        <v>2</v>
-      </c>
       <c r="H14" t="s">
-        <v>1</v>
-      </c>
-      <c r="I14" s="1" t="s">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="15" spans="1:9">
+        <v>2</v>
+      </c>
+      <c r="I14" t="s">
+        <v>1</v>
+      </c>
+      <c r="J14" s="1" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="15" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A15">
         <v>52</v>
       </c>
-      <c r="B15" t="s">
+      <c r="B15">
+        <v>710</v>
+      </c>
+      <c r="C15" t="s">
         <v>15</v>
       </c>
-      <c r="C15" t="s">
+      <c r="D15" t="s">
         <v>27</v>
       </c>
-      <c r="D15" t="s">
+      <c r="E15" t="s">
         <v>24</v>
       </c>
-      <c r="E15">
+      <c r="F15">
         <v>518</v>
       </c>
-      <c r="F15" t="s">
+      <c r="G15" t="s">
         <v>13</v>
       </c>
-      <c r="G15" t="s">
-        <v>2</v>
-      </c>
       <c r="H15" t="s">
-        <v>1</v>
-      </c>
-      <c r="I15" s="1" t="s">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="16" spans="1:9">
+        <v>2</v>
+      </c>
+      <c r="I15" t="s">
+        <v>1</v>
+      </c>
+      <c r="J15" s="1" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="16" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A16">
         <v>8</v>
       </c>
-      <c r="B16" t="s">
-        <v>6</v>
+      <c r="B16">
+        <v>715</v>
       </c>
       <c r="C16" t="s">
+        <v>6</v>
+      </c>
+      <c r="D16" t="s">
         <v>26</v>
       </c>
-      <c r="D16" t="s">
+      <c r="E16" t="s">
         <v>24</v>
       </c>
-      <c r="E16">
+      <c r="F16">
         <v>518</v>
       </c>
-      <c r="F16" t="s">
-        <v>3</v>
-      </c>
       <c r="G16" t="s">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="H16" t="s">
-        <v>1</v>
-      </c>
-      <c r="I16" s="1" t="s">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="17" spans="1:9">
+        <v>2</v>
+      </c>
+      <c r="I16" t="s">
+        <v>1</v>
+      </c>
+      <c r="J16" s="1" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="17" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A17">
         <v>51</v>
       </c>
-      <c r="B17" t="s">
-        <v>6</v>
+      <c r="B17">
+        <v>715</v>
       </c>
       <c r="C17" t="s">
+        <v>6</v>
+      </c>
+      <c r="D17" t="s">
         <v>25</v>
       </c>
-      <c r="D17" t="s">
+      <c r="E17" t="s">
         <v>24</v>
       </c>
-      <c r="E17">
+      <c r="F17">
         <v>518</v>
       </c>
-      <c r="F17" t="s">
-        <v>3</v>
-      </c>
       <c r="G17" t="s">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="H17" t="s">
-        <v>1</v>
-      </c>
-      <c r="I17" s="1" t="s">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="18" spans="1:9">
+        <v>2</v>
+      </c>
+      <c r="I17" t="s">
+        <v>1</v>
+      </c>
+      <c r="J17" s="1" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="18" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A18">
         <v>61</v>
       </c>
-      <c r="B18" t="s">
+      <c r="B18">
+        <v>719</v>
+      </c>
+      <c r="C18" t="s">
         <v>15</v>
       </c>
-      <c r="C18" t="s">
+      <c r="D18" t="s">
         <v>23</v>
       </c>
-      <c r="D18" t="s">
+      <c r="E18" t="s">
         <v>19</v>
       </c>
-      <c r="E18">
+      <c r="F18">
         <v>531</v>
       </c>
-      <c r="F18" t="s">
+      <c r="G18" t="s">
         <v>13</v>
       </c>
-      <c r="G18" t="s">
-        <v>2</v>
-      </c>
       <c r="H18" t="s">
-        <v>1</v>
-      </c>
-      <c r="I18" s="1" t="s">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="19" spans="1:9">
+        <v>2</v>
+      </c>
+      <c r="I18" t="s">
+        <v>1</v>
+      </c>
+      <c r="J18" s="1" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="19" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A19">
         <v>60</v>
       </c>
-      <c r="B19" t="s">
+      <c r="B19">
+        <v>719</v>
+      </c>
+      <c r="C19" t="s">
         <v>15</v>
       </c>
-      <c r="C19" t="s">
+      <c r="D19" t="s">
         <v>22</v>
       </c>
-      <c r="D19" t="s">
+      <c r="E19" t="s">
         <v>19</v>
       </c>
-      <c r="E19">
+      <c r="F19">
         <v>531</v>
       </c>
-      <c r="F19" t="s">
+      <c r="G19" t="s">
         <v>13</v>
       </c>
-      <c r="G19" t="s">
-        <v>2</v>
-      </c>
       <c r="H19" t="s">
-        <v>1</v>
-      </c>
-      <c r="I19" s="1" t="s">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="20" spans="1:9">
+        <v>2</v>
+      </c>
+      <c r="I19" t="s">
+        <v>1</v>
+      </c>
+      <c r="J19" s="1" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="20" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A20">
         <v>59</v>
       </c>
-      <c r="B20" t="s">
-        <v>6</v>
+      <c r="B20">
+        <v>720</v>
       </c>
       <c r="C20" t="s">
+        <v>6</v>
+      </c>
+      <c r="D20" t="s">
         <v>21</v>
       </c>
-      <c r="D20" t="s">
+      <c r="E20" t="s">
         <v>19</v>
       </c>
-      <c r="E20">
+      <c r="F20">
         <v>531</v>
       </c>
-      <c r="F20" t="s">
-        <v>3</v>
-      </c>
       <c r="G20" t="s">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="H20" t="s">
-        <v>1</v>
-      </c>
-      <c r="I20" s="1" t="s">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="21" spans="1:9">
+        <v>2</v>
+      </c>
+      <c r="I20" t="s">
+        <v>1</v>
+      </c>
+      <c r="J20" s="1" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="21" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A21">
         <v>58</v>
       </c>
-      <c r="B21" t="s">
-        <v>6</v>
+      <c r="B21">
+        <v>720</v>
       </c>
       <c r="C21" t="s">
+        <v>6</v>
+      </c>
+      <c r="D21" t="s">
         <v>20</v>
       </c>
-      <c r="D21" t="s">
+      <c r="E21" t="s">
         <v>19</v>
       </c>
-      <c r="E21">
+      <c r="F21">
         <v>531</v>
       </c>
-      <c r="F21" s="1" t="s">
-        <v>3</v>
-      </c>
-      <c r="G21" t="s">
-        <v>2</v>
+      <c r="G21" s="1" t="s">
+        <v>3</v>
       </c>
       <c r="H21" t="s">
-        <v>1</v>
-      </c>
-      <c r="I21" s="1" t="s">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="22" spans="1:9">
+        <v>2</v>
+      </c>
+      <c r="I21" t="s">
+        <v>1</v>
+      </c>
+      <c r="J21" s="1" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="22" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A22">
         <v>69</v>
       </c>
-      <c r="B22" t="s">
-        <v>6</v>
+      <c r="B22">
+        <v>722</v>
       </c>
       <c r="C22" t="s">
+        <v>6</v>
+      </c>
+      <c r="D22" t="s">
         <v>18</v>
       </c>
-      <c r="D22" t="s">
-        <v>4</v>
-      </c>
-      <c r="E22">
+      <c r="E22" t="s">
+        <v>4</v>
+      </c>
+      <c r="F22">
         <v>532</v>
       </c>
-      <c r="F22" s="1" t="s">
-        <v>3</v>
-      </c>
-      <c r="G22" t="s">
-        <v>2</v>
+      <c r="G22" s="1" t="s">
+        <v>3</v>
       </c>
       <c r="H22" t="s">
-        <v>1</v>
-      </c>
-      <c r="I22" s="1" t="s">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="23" spans="1:9">
+        <v>2</v>
+      </c>
+      <c r="I22" t="s">
+        <v>1</v>
+      </c>
+      <c r="J22" s="1" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="23" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A23">
         <v>74</v>
       </c>
-      <c r="B23" t="s">
-        <v>6</v>
+      <c r="B23">
+        <v>722</v>
       </c>
       <c r="C23" t="s">
+        <v>6</v>
+      </c>
+      <c r="D23" t="s">
         <v>17</v>
       </c>
-      <c r="D23" t="s">
-        <v>4</v>
-      </c>
-      <c r="E23">
+      <c r="E23" t="s">
+        <v>4</v>
+      </c>
+      <c r="F23">
         <v>532</v>
       </c>
-      <c r="F23" s="1" t="s">
-        <v>3</v>
-      </c>
-      <c r="G23" t="s">
-        <v>2</v>
+      <c r="G23" s="1" t="s">
+        <v>3</v>
       </c>
       <c r="H23" t="s">
-        <v>1</v>
-      </c>
-      <c r="I23" s="1" t="s">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="24" spans="1:9">
+        <v>2</v>
+      </c>
+      <c r="I23" t="s">
+        <v>1</v>
+      </c>
+      <c r="J23" s="1" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="24" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A24">
         <v>47</v>
       </c>
-      <c r="B24" t="s">
+      <c r="B24">
+        <v>711</v>
+      </c>
+      <c r="C24" t="s">
         <v>15</v>
       </c>
-      <c r="C24" t="s">
+      <c r="D24" t="s">
         <v>16</v>
       </c>
-      <c r="D24" t="s">
-        <v>4</v>
-      </c>
-      <c r="E24">
+      <c r="E24" t="s">
+        <v>4</v>
+      </c>
+      <c r="F24">
         <v>529</v>
       </c>
-      <c r="F24" t="s">
+      <c r="G24" t="s">
         <v>13</v>
       </c>
-      <c r="G24" t="s">
-        <v>2</v>
-      </c>
       <c r="H24" t="s">
-        <v>1</v>
-      </c>
-      <c r="I24" s="1" t="s">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="25" spans="1:9">
+        <v>2</v>
+      </c>
+      <c r="I24" t="s">
+        <v>1</v>
+      </c>
+      <c r="J24" s="1" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="25" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A25">
         <v>53</v>
       </c>
-      <c r="B25" t="s">
+      <c r="B25">
+        <v>711</v>
+      </c>
+      <c r="C25" t="s">
         <v>15</v>
       </c>
-      <c r="C25" t="s">
+      <c r="D25" t="s">
         <v>14</v>
       </c>
-      <c r="D25" t="s">
-        <v>4</v>
-      </c>
-      <c r="E25">
+      <c r="E25" t="s">
+        <v>4</v>
+      </c>
+      <c r="F25">
         <v>529</v>
       </c>
-      <c r="F25" t="s">
+      <c r="G25" t="s">
         <v>13</v>
       </c>
-      <c r="G25" t="s">
-        <v>2</v>
-      </c>
       <c r="H25" t="s">
-        <v>1</v>
-      </c>
-      <c r="I25" s="1" t="s">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="26" spans="1:9">
+        <v>2</v>
+      </c>
+      <c r="I25" t="s">
+        <v>1</v>
+      </c>
+      <c r="J25" s="1" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="26" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A26">
         <v>12</v>
       </c>
-      <c r="B26" t="s">
-        <v>6</v>
+      <c r="B26">
+        <v>718</v>
       </c>
       <c r="C26" t="s">
+        <v>6</v>
+      </c>
+      <c r="D26" t="s">
         <v>12</v>
       </c>
-      <c r="D26" t="s">
-        <v>4</v>
-      </c>
-      <c r="E26">
+      <c r="E26" t="s">
+        <v>4</v>
+      </c>
+      <c r="F26">
         <v>529</v>
       </c>
-      <c r="F26" s="1" t="s">
-        <v>3</v>
-      </c>
-      <c r="G26" t="s">
-        <v>2</v>
+      <c r="G26" s="1" t="s">
+        <v>3</v>
       </c>
       <c r="H26" t="s">
-        <v>1</v>
-      </c>
-      <c r="I26" s="1" t="s">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="27" spans="1:9">
+        <v>2</v>
+      </c>
+      <c r="I26" t="s">
+        <v>1</v>
+      </c>
+      <c r="J26" s="1" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="27" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A27">
         <v>9</v>
       </c>
-      <c r="B27" t="s">
-        <v>6</v>
+      <c r="B27">
+        <v>718</v>
       </c>
       <c r="C27" t="s">
+        <v>6</v>
+      </c>
+      <c r="D27" t="s">
         <v>11</v>
       </c>
-      <c r="D27" t="s">
-        <v>4</v>
-      </c>
-      <c r="E27">
+      <c r="E27" t="s">
+        <v>4</v>
+      </c>
+      <c r="F27">
         <v>529</v>
       </c>
-      <c r="F27" s="1" t="s">
-        <v>3</v>
-      </c>
-      <c r="G27" t="s">
-        <v>2</v>
+      <c r="G27" s="1" t="s">
+        <v>3</v>
       </c>
       <c r="H27" t="s">
-        <v>1</v>
-      </c>
-      <c r="I27" s="1" t="s">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="28" spans="1:9">
+        <v>2</v>
+      </c>
+      <c r="I27" t="s">
+        <v>1</v>
+      </c>
+      <c r="J27" s="1" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="28" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A28">
         <v>68</v>
       </c>
-      <c r="B28" t="s">
-        <v>6</v>
+      <c r="B28">
+        <v>721</v>
       </c>
       <c r="C28" t="s">
+        <v>6</v>
+      </c>
+      <c r="D28" t="s">
         <v>10</v>
       </c>
-      <c r="D28" t="s">
-        <v>4</v>
-      </c>
-      <c r="E28">
+      <c r="E28" t="s">
+        <v>4</v>
+      </c>
+      <c r="F28">
         <v>352</v>
       </c>
-      <c r="F28" s="1" t="s">
-        <v>3</v>
-      </c>
-      <c r="G28" t="s">
-        <v>2</v>
+      <c r="G28" s="1" t="s">
+        <v>3</v>
       </c>
       <c r="H28" t="s">
-        <v>1</v>
-      </c>
-      <c r="I28" s="1" t="s">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="29" spans="1:9">
+        <v>2</v>
+      </c>
+      <c r="I28" t="s">
+        <v>1</v>
+      </c>
+      <c r="J28" s="1" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="29" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A29">
         <v>73</v>
       </c>
-      <c r="B29" t="s">
-        <v>6</v>
+      <c r="B29">
+        <v>721</v>
       </c>
       <c r="C29" t="s">
+        <v>6</v>
+      </c>
+      <c r="D29" t="s">
         <v>9</v>
       </c>
-      <c r="D29" t="s">
-        <v>4</v>
-      </c>
-      <c r="E29">
+      <c r="E29" t="s">
+        <v>4</v>
+      </c>
+      <c r="F29">
         <v>352</v>
       </c>
-      <c r="F29" s="1" t="s">
-        <v>3</v>
-      </c>
-      <c r="G29" t="s">
-        <v>2</v>
+      <c r="G29" s="1" t="s">
+        <v>3</v>
       </c>
       <c r="H29" t="s">
-        <v>1</v>
-      </c>
-      <c r="I29" s="1" t="s">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="30" spans="1:9">
+        <v>2</v>
+      </c>
+      <c r="I29" t="s">
+        <v>1</v>
+      </c>
+      <c r="J29" s="1" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="30" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A30">
         <v>71</v>
       </c>
-      <c r="B30" t="s">
-        <v>6</v>
+      <c r="B30">
+        <v>724</v>
       </c>
       <c r="C30" t="s">
+        <v>6</v>
+      </c>
+      <c r="D30" t="s">
         <v>8</v>
       </c>
-      <c r="D30" t="s">
-        <v>4</v>
-      </c>
-      <c r="E30">
+      <c r="E30" t="s">
+        <v>4</v>
+      </c>
+      <c r="F30">
         <v>534</v>
       </c>
-      <c r="F30" s="1" t="s">
-        <v>3</v>
-      </c>
-      <c r="G30" t="s">
-        <v>2</v>
+      <c r="G30" s="1" t="s">
+        <v>3</v>
       </c>
       <c r="H30" t="s">
-        <v>1</v>
-      </c>
-      <c r="I30" s="1" t="s">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="31" spans="1:9">
+        <v>2</v>
+      </c>
+      <c r="I30" t="s">
+        <v>1</v>
+      </c>
+      <c r="J30" s="1" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="31" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A31">
         <v>70</v>
       </c>
-      <c r="B31" t="s">
-        <v>6</v>
+      <c r="B31">
+        <v>723</v>
       </c>
       <c r="C31" t="s">
+        <v>6</v>
+      </c>
+      <c r="D31" t="s">
         <v>7</v>
       </c>
-      <c r="D31" t="s">
-        <v>4</v>
-      </c>
-      <c r="E31">
+      <c r="E31" t="s">
+        <v>4</v>
+      </c>
+      <c r="F31">
         <v>533</v>
       </c>
-      <c r="F31" s="1" t="s">
-        <v>3</v>
-      </c>
-      <c r="G31" t="s">
-        <v>2</v>
+      <c r="G31" s="1" t="s">
+        <v>3</v>
       </c>
       <c r="H31" t="s">
-        <v>1</v>
-      </c>
-      <c r="I31" s="1" t="s">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="32" spans="1:9">
+        <v>2</v>
+      </c>
+      <c r="I31" t="s">
+        <v>1</v>
+      </c>
+      <c r="J31" s="1" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="32" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A32">
         <v>75</v>
       </c>
-      <c r="B32" t="s">
-        <v>6</v>
+      <c r="B32">
+        <v>723</v>
       </c>
       <c r="C32" t="s">
+        <v>6</v>
+      </c>
+      <c r="D32" t="s">
         <v>5</v>
       </c>
-      <c r="D32" t="s">
-        <v>4</v>
-      </c>
-      <c r="E32">
+      <c r="E32" t="s">
+        <v>4</v>
+      </c>
+      <c r="F32">
         <v>533</v>
       </c>
-      <c r="F32" s="1" t="s">
-        <v>3</v>
-      </c>
-      <c r="G32" t="s">
-        <v>2</v>
+      <c r="G32" s="1" t="s">
+        <v>3</v>
       </c>
       <c r="H32" t="s">
-        <v>1</v>
-      </c>
-      <c r="I32" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="I32" t="s">
+        <v>1</v>
+      </c>
+      <c r="J32" s="1" t="s">
         <v>0</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
-  <extLst>
-    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
-      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
-    </ext>
-  </extLst>
 </worksheet>
 </file>
</xml_diff>